<commit_message>
Converted to TestNG format
</commit_message>
<xml_diff>
--- a/Data/Jenkin.xlsx
+++ b/Data/Jenkin.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
   <si>
     <t>Input</t>
   </si>
@@ -1033,29 +1033,29 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>13</v>
-      </c>
-      <c r="K2">
-        <v>21</v>
-      </c>
-      <c r="L2">
-        <v>34</v>
+      <c r="E2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>34.0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1071,14 +1071,14 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1108,11 +1108,11 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>